<commit_message>
This commit updates the column name 'ensemble_decision' to 'mdsgene_decision' across multiple modules to ensure consistency with the data structure. It also includes renaming column in the Excel files in the 'excel' directory.
</commit_message>
<xml_diff>
--- a/excel/GBA-GD-DLB.xlsx
+++ b/excel/GBA-GD-DLB.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\madoev\Desktop\Nairi-New7\MDSGene_backend\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142E49CA-9184-46D1-A5E0-134B56A5B7E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="19440"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -509,9 +515,6 @@
     <t>functional_evidence3</t>
   </si>
   <si>
-    <t>ensemble_decision</t>
-  </si>
-  <si>
     <t>comment decision</t>
   </si>
   <si>
@@ -753,19 +756,16 @@
   </si>
   <si>
     <t>ISR</t>
+  </si>
+  <si>
+    <t>mdsgene_decision</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-  </numFmts>
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -781,353 +781,16 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1150,251 +813,9 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1402,61 +823,17 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Percent" xfId="3" builtinId="5"/>
-    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
-    <cellStyle name="Note" xfId="8" builtinId="10"/>
-    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
-    <cellStyle name="Title" xfId="10" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
-    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
-    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
-    <cellStyle name="Input" xfId="16" builtinId="20"/>
-    <cellStyle name="Output" xfId="17" builtinId="21"/>
-    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
-    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
-    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
-    <cellStyle name="Total" xfId="21" builtinId="25"/>
-    <cellStyle name="Good" xfId="22" builtinId="26"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1741,21 +1118,21 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:FG10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3:K10"/>
+    <sheetView tabSelected="1" topLeftCell="EQ1" workbookViewId="0">
+      <selection activeCell="FE1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="11" max="11" width="11.4609375" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:163">
@@ -2240,13 +1617,13 @@
         <v>159</v>
       </c>
       <c r="FE1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="FF1" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="FF1" s="1" t="s">
+      <c r="FG1" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="FG1" s="1" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:163">
@@ -2254,34 +1631,34 @@
         <v>29595653</v>
       </c>
       <c r="B2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" t="s">
         <v>163</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2">
+        <v>-99</v>
+      </c>
+      <c r="E2">
+        <v>-99</v>
+      </c>
+      <c r="F2">
+        <v>-99</v>
+      </c>
+      <c r="G2">
+        <v>-99</v>
+      </c>
+      <c r="H2" t="s">
         <v>164</v>
       </c>
-      <c r="D2">
-        <v>-99</v>
-      </c>
-      <c r="E2">
-        <v>-99</v>
-      </c>
-      <c r="F2">
-        <v>-99</v>
-      </c>
-      <c r="G2">
-        <v>-99</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>165</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
+        <v>165</v>
+      </c>
+      <c r="K2" t="s">
         <v>166</v>
-      </c>
-      <c r="J2" t="s">
-        <v>166</v>
-      </c>
-      <c r="K2" t="s">
-        <v>167</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -2293,13 +1670,13 @@
         <v>-99</v>
       </c>
       <c r="O2" t="s">
+        <v>167</v>
+      </c>
+      <c r="P2" t="s">
         <v>168</v>
       </c>
-      <c r="P2" t="s">
-        <v>169</v>
-      </c>
       <c r="Q2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="R2">
         <v>-99</v>
@@ -2323,7 +1700,7 @@
         <v>-99</v>
       </c>
       <c r="Y2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Z2">
         <v>62</v>
@@ -2350,364 +1727,364 @@
         <v>19</v>
       </c>
       <c r="AH2" t="s">
+        <v>171</v>
+      </c>
+      <c r="AI2" t="s">
         <v>172</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>173</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>174</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AL2" t="s">
         <v>175</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AM2" t="s">
         <v>176</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AN2" t="s">
         <v>177</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AO2" t="s">
         <v>178</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AP2" t="s">
         <v>179</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AQ2" t="s">
         <v>180</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="AR2" t="s">
         <v>181</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AS2" t="s">
         <v>182</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AT2">
+        <v>-99</v>
+      </c>
+      <c r="AU2" t="s">
         <v>183</v>
       </c>
-      <c r="AT2">
-        <v>-99</v>
-      </c>
-      <c r="AU2" t="s">
+      <c r="AV2" t="s">
+        <v>171</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>172</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>173</v>
+      </c>
+      <c r="AY2" t="s">
         <v>184</v>
       </c>
-      <c r="AV2" t="s">
-        <v>172</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>173</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>174</v>
-      </c>
-      <c r="AY2" t="s">
+      <c r="AZ2" t="s">
+        <v>176</v>
+      </c>
+      <c r="BA2" t="s">
         <v>185</v>
       </c>
-      <c r="AZ2" t="s">
-        <v>177</v>
-      </c>
-      <c r="BA2" t="s">
+      <c r="BB2" t="s">
         <v>186</v>
       </c>
-      <c r="BB2" t="s">
+      <c r="BC2" t="s">
         <v>187</v>
       </c>
-      <c r="BC2" t="s">
+      <c r="BD2" t="s">
         <v>188</v>
       </c>
-      <c r="BD2" t="s">
+      <c r="BE2" t="s">
         <v>189</v>
       </c>
-      <c r="BE2" t="s">
+      <c r="BF2" t="s">
+        <v>181</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>182</v>
+      </c>
+      <c r="BH2">
+        <v>-99</v>
+      </c>
+      <c r="BI2">
+        <v>-99</v>
+      </c>
+      <c r="BJ2">
+        <v>-99</v>
+      </c>
+      <c r="BK2">
+        <v>-99</v>
+      </c>
+      <c r="BL2">
+        <v>-99</v>
+      </c>
+      <c r="BM2">
+        <v>-99</v>
+      </c>
+      <c r="BN2">
+        <v>-99</v>
+      </c>
+      <c r="BO2">
+        <v>-99</v>
+      </c>
+      <c r="BP2">
+        <v>-99</v>
+      </c>
+      <c r="BQ2">
+        <v>-99</v>
+      </c>
+      <c r="BR2">
+        <v>-99</v>
+      </c>
+      <c r="BS2">
+        <v>-99</v>
+      </c>
+      <c r="BT2" t="s">
         <v>190</v>
       </c>
-      <c r="BF2" t="s">
-        <v>182</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>183</v>
-      </c>
-      <c r="BH2">
-        <v>-99</v>
-      </c>
-      <c r="BI2">
-        <v>-99</v>
-      </c>
-      <c r="BJ2">
-        <v>-99</v>
-      </c>
-      <c r="BK2">
-        <v>-99</v>
-      </c>
-      <c r="BL2">
-        <v>-99</v>
-      </c>
-      <c r="BM2">
-        <v>-99</v>
-      </c>
-      <c r="BN2">
-        <v>-99</v>
-      </c>
-      <c r="BO2">
-        <v>-99</v>
-      </c>
-      <c r="BP2">
-        <v>-99</v>
-      </c>
-      <c r="BQ2">
-        <v>-99</v>
-      </c>
-      <c r="BR2">
-        <v>-99</v>
-      </c>
-      <c r="BS2">
-        <v>-99</v>
-      </c>
-      <c r="BT2" t="s">
+      <c r="BU2">
+        <v>-99</v>
+      </c>
+      <c r="BV2">
+        <v>-99</v>
+      </c>
+      <c r="BW2">
+        <v>-99</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>169</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>169</v>
+      </c>
+      <c r="BZ2" t="s">
         <v>191</v>
       </c>
-      <c r="BU2">
-        <v>-99</v>
-      </c>
-      <c r="BV2">
-        <v>-99</v>
-      </c>
-      <c r="BW2">
-        <v>-99</v>
-      </c>
-      <c r="BX2" t="s">
-        <v>170</v>
-      </c>
-      <c r="BY2" t="s">
-        <v>170</v>
-      </c>
-      <c r="BZ2" t="s">
+      <c r="CA2">
+        <v>-99</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>169</v>
+      </c>
+      <c r="CC2">
+        <v>-99</v>
+      </c>
+      <c r="CD2">
+        <v>-99</v>
+      </c>
+      <c r="CE2">
+        <v>-99</v>
+      </c>
+      <c r="CF2">
+        <v>-99</v>
+      </c>
+      <c r="CG2" t="s">
+        <v>169</v>
+      </c>
+      <c r="CH2" t="s">
+        <v>169</v>
+      </c>
+      <c r="CI2">
+        <v>-99</v>
+      </c>
+      <c r="CJ2">
+        <v>-99</v>
+      </c>
+      <c r="CK2">
+        <v>-99</v>
+      </c>
+      <c r="CL2">
+        <v>-99</v>
+      </c>
+      <c r="CM2">
+        <v>-99</v>
+      </c>
+      <c r="CN2">
+        <v>-99</v>
+      </c>
+      <c r="CO2">
+        <v>-99</v>
+      </c>
+      <c r="CP2">
+        <v>-99</v>
+      </c>
+      <c r="CQ2">
+        <v>-99</v>
+      </c>
+      <c r="CR2">
+        <v>-99</v>
+      </c>
+      <c r="CS2">
+        <v>-99</v>
+      </c>
+      <c r="CT2">
+        <v>-99</v>
+      </c>
+      <c r="CU2" t="s">
+        <v>169</v>
+      </c>
+      <c r="CV2">
+        <v>-99</v>
+      </c>
+      <c r="CW2">
+        <v>-99</v>
+      </c>
+      <c r="CX2">
+        <v>-99</v>
+      </c>
+      <c r="CY2" t="s">
+        <v>169</v>
+      </c>
+      <c r="CZ2" t="s">
+        <v>169</v>
+      </c>
+      <c r="DA2">
+        <v>-99</v>
+      </c>
+      <c r="DB2" t="s">
+        <v>169</v>
+      </c>
+      <c r="DC2">
+        <v>-99</v>
+      </c>
+      <c r="DD2">
+        <v>-99</v>
+      </c>
+      <c r="DE2">
+        <v>-99</v>
+      </c>
+      <c r="DF2">
+        <v>-99</v>
+      </c>
+      <c r="DG2">
+        <v>-99</v>
+      </c>
+      <c r="DH2">
+        <v>-99</v>
+      </c>
+      <c r="DI2">
+        <v>-99</v>
+      </c>
+      <c r="DJ2">
+        <v>-99</v>
+      </c>
+      <c r="DK2">
+        <v>-99</v>
+      </c>
+      <c r="DL2">
+        <v>-99</v>
+      </c>
+      <c r="DM2" t="s">
+        <v>169</v>
+      </c>
+      <c r="DN2">
+        <v>-99</v>
+      </c>
+      <c r="DO2">
+        <v>-99</v>
+      </c>
+      <c r="DP2">
+        <v>-99</v>
+      </c>
+      <c r="DQ2">
+        <v>-99</v>
+      </c>
+      <c r="DR2">
+        <v>-99</v>
+      </c>
+      <c r="DS2">
+        <v>-99</v>
+      </c>
+      <c r="DT2" t="s">
+        <v>169</v>
+      </c>
+      <c r="DU2" t="s">
         <v>192</v>
       </c>
-      <c r="CA2">
-        <v>-99</v>
-      </c>
-      <c r="CB2" t="s">
-        <v>170</v>
-      </c>
-      <c r="CC2">
-        <v>-99</v>
-      </c>
-      <c r="CD2">
-        <v>-99</v>
-      </c>
-      <c r="CE2">
-        <v>-99</v>
-      </c>
-      <c r="CF2">
-        <v>-99</v>
-      </c>
-      <c r="CG2" t="s">
-        <v>170</v>
-      </c>
-      <c r="CH2" t="s">
-        <v>170</v>
-      </c>
-      <c r="CI2">
-        <v>-99</v>
-      </c>
-      <c r="CJ2">
-        <v>-99</v>
-      </c>
-      <c r="CK2">
-        <v>-99</v>
-      </c>
-      <c r="CL2">
-        <v>-99</v>
-      </c>
-      <c r="CM2">
-        <v>-99</v>
-      </c>
-      <c r="CN2">
-        <v>-99</v>
-      </c>
-      <c r="CO2">
-        <v>-99</v>
-      </c>
-      <c r="CP2">
-        <v>-99</v>
-      </c>
-      <c r="CQ2">
-        <v>-99</v>
-      </c>
-      <c r="CR2">
-        <v>-99</v>
-      </c>
-      <c r="CS2">
-        <v>-99</v>
-      </c>
-      <c r="CT2">
-        <v>-99</v>
-      </c>
-      <c r="CU2" t="s">
-        <v>170</v>
-      </c>
-      <c r="CV2">
-        <v>-99</v>
-      </c>
-      <c r="CW2">
-        <v>-99</v>
-      </c>
-      <c r="CX2">
-        <v>-99</v>
-      </c>
-      <c r="CY2" t="s">
-        <v>170</v>
-      </c>
-      <c r="CZ2" t="s">
-        <v>170</v>
-      </c>
-      <c r="DA2">
-        <v>-99</v>
-      </c>
-      <c r="DB2" t="s">
-        <v>170</v>
-      </c>
-      <c r="DC2">
-        <v>-99</v>
-      </c>
-      <c r="DD2">
-        <v>-99</v>
-      </c>
-      <c r="DE2">
-        <v>-99</v>
-      </c>
-      <c r="DF2">
-        <v>-99</v>
-      </c>
-      <c r="DG2">
-        <v>-99</v>
-      </c>
-      <c r="DH2">
-        <v>-99</v>
-      </c>
-      <c r="DI2">
-        <v>-99</v>
-      </c>
-      <c r="DJ2">
-        <v>-99</v>
-      </c>
-      <c r="DK2">
-        <v>-99</v>
-      </c>
-      <c r="DL2">
-        <v>-99</v>
-      </c>
-      <c r="DM2" t="s">
-        <v>170</v>
-      </c>
-      <c r="DN2">
-        <v>-99</v>
-      </c>
-      <c r="DO2">
-        <v>-99</v>
-      </c>
-      <c r="DP2">
-        <v>-99</v>
-      </c>
-      <c r="DQ2">
-        <v>-99</v>
-      </c>
-      <c r="DR2">
-        <v>-99</v>
-      </c>
-      <c r="DS2">
-        <v>-99</v>
-      </c>
-      <c r="DT2" t="s">
-        <v>170</v>
-      </c>
-      <c r="DU2" t="s">
+      <c r="DV2">
+        <v>-99</v>
+      </c>
+      <c r="DW2">
+        <v>-99</v>
+      </c>
+      <c r="DX2">
+        <v>-99</v>
+      </c>
+      <c r="DY2">
+        <v>-99</v>
+      </c>
+      <c r="DZ2" t="s">
         <v>193</v>
       </c>
-      <c r="DV2">
-        <v>-99</v>
-      </c>
-      <c r="DW2">
-        <v>-99</v>
-      </c>
-      <c r="DX2">
-        <v>-99</v>
-      </c>
-      <c r="DY2">
-        <v>-99</v>
-      </c>
-      <c r="DZ2" t="s">
+      <c r="EA2">
+        <v>-99</v>
+      </c>
+      <c r="EB2">
+        <v>-99</v>
+      </c>
+      <c r="EC2">
+        <v>-99</v>
+      </c>
+      <c r="ED2" t="s">
         <v>194</v>
       </c>
-      <c r="EA2">
-        <v>-99</v>
-      </c>
-      <c r="EB2">
-        <v>-99</v>
-      </c>
-      <c r="EC2">
-        <v>-99</v>
-      </c>
-      <c r="ED2" t="s">
+      <c r="EE2" t="s">
         <v>195</v>
       </c>
-      <c r="EE2" t="s">
+      <c r="EF2">
+        <v>-99</v>
+      </c>
+      <c r="EG2" t="s">
         <v>196</v>
       </c>
-      <c r="EF2">
-        <v>-99</v>
-      </c>
-      <c r="EG2" t="s">
+      <c r="EH2" t="s">
+        <v>195</v>
+      </c>
+      <c r="EI2">
+        <v>-99</v>
+      </c>
+      <c r="EJ2" t="s">
+        <v>196</v>
+      </c>
+      <c r="EK2" t="s">
+        <v>195</v>
+      </c>
+      <c r="EL2">
+        <v>-99</v>
+      </c>
+      <c r="EM2" t="s">
         <v>197</v>
       </c>
-      <c r="EH2" t="s">
+      <c r="EN2" t="s">
+        <v>198</v>
+      </c>
+      <c r="EO2">
+        <v>-99</v>
+      </c>
+      <c r="EP2" t="s">
         <v>196</v>
       </c>
-      <c r="EI2">
-        <v>-99</v>
-      </c>
-      <c r="EJ2" t="s">
-        <v>197</v>
-      </c>
-      <c r="EK2" t="s">
-        <v>196</v>
-      </c>
-      <c r="EL2">
-        <v>-99</v>
-      </c>
-      <c r="EM2" t="s">
-        <v>198</v>
-      </c>
-      <c r="EN2" t="s">
+      <c r="EQ2" t="s">
+        <v>195</v>
+      </c>
+      <c r="ER2">
+        <v>-99</v>
+      </c>
+      <c r="ES2" t="s">
         <v>199</v>
       </c>
-      <c r="EO2">
-        <v>-99</v>
-      </c>
-      <c r="EP2" t="s">
-        <v>197</v>
-      </c>
-      <c r="EQ2" t="s">
-        <v>196</v>
-      </c>
-      <c r="ER2">
-        <v>-99</v>
-      </c>
-      <c r="ES2" t="s">
+      <c r="ET2" t="s">
         <v>200</v>
       </c>
-      <c r="ET2" t="s">
+      <c r="EU2">
+        <v>-99</v>
+      </c>
+      <c r="EV2" t="s">
         <v>201</v>
       </c>
-      <c r="EU2">
-        <v>-99</v>
-      </c>
-      <c r="EV2" t="s">
+      <c r="EW2" t="s">
         <v>202</v>
-      </c>
-      <c r="EW2" t="s">
-        <v>203</v>
       </c>
       <c r="EX2">
         <v>-99</v>
@@ -2722,16 +2099,16 @@
         <v>-99</v>
       </c>
       <c r="FB2" t="s">
+        <v>203</v>
+      </c>
+      <c r="FC2" t="s">
         <v>204</v>
       </c>
-      <c r="FC2" t="s">
+      <c r="FD2">
+        <v>-99</v>
+      </c>
+      <c r="FE2" t="s">
         <v>205</v>
-      </c>
-      <c r="FD2">
-        <v>-99</v>
-      </c>
-      <c r="FE2" t="s">
-        <v>206</v>
       </c>
       <c r="FF2">
         <v>-99</v>
@@ -2745,34 +2122,34 @@
         <v>21742527</v>
       </c>
       <c r="B3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C3" t="s">
         <v>207</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>208</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3">
+        <v>-99</v>
+      </c>
+      <c r="F3">
+        <v>-99</v>
+      </c>
+      <c r="G3">
+        <v>-99</v>
+      </c>
+      <c r="H3">
+        <v>-99</v>
+      </c>
+      <c r="I3" t="s">
         <v>209</v>
-      </c>
-      <c r="E3">
-        <v>-99</v>
-      </c>
-      <c r="F3">
-        <v>-99</v>
-      </c>
-      <c r="G3">
-        <v>-99</v>
-      </c>
-      <c r="H3">
-        <v>-99</v>
-      </c>
-      <c r="I3" t="s">
-        <v>210</v>
       </c>
       <c r="J3">
         <v>16</v>
       </c>
       <c r="K3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L3">
         <v>-99</v>
@@ -2784,13 +2161,13 @@
         <v>-99</v>
       </c>
       <c r="O3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="P3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="Q3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="R3">
         <v>-99</v>
@@ -2814,7 +2191,7 @@
         <v>-99</v>
       </c>
       <c r="Y3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Z3">
         <v>-99</v>
@@ -2841,46 +2218,46 @@
         <v>19</v>
       </c>
       <c r="AH3" t="s">
+        <v>171</v>
+      </c>
+      <c r="AI3" t="s">
         <v>172</v>
       </c>
-      <c r="AI3" t="s">
+      <c r="AJ3" t="s">
         <v>173</v>
       </c>
-      <c r="AJ3" t="s">
+      <c r="AK3" t="s">
         <v>174</v>
       </c>
-      <c r="AK3" t="s">
+      <c r="AL3" t="s">
         <v>175</v>
       </c>
-      <c r="AL3" t="s">
+      <c r="AM3" t="s">
         <v>176</v>
       </c>
-      <c r="AM3" t="s">
+      <c r="AN3" t="s">
         <v>177</v>
       </c>
-      <c r="AN3" t="s">
+      <c r="AO3" t="s">
         <v>178</v>
       </c>
-      <c r="AO3" t="s">
+      <c r="AP3" t="s">
         <v>179</v>
       </c>
-      <c r="AP3" t="s">
+      <c r="AQ3" t="s">
         <v>180</v>
       </c>
-      <c r="AQ3" t="s">
-        <v>181</v>
-      </c>
       <c r="AR3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AS3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AT3">
         <v>-99</v>
       </c>
       <c r="AU3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AV3">
         <v>-99</v>
@@ -2916,7 +2293,7 @@
         <v>-99</v>
       </c>
       <c r="BG3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="BH3">
         <v>-99</v>
@@ -2955,7 +2332,7 @@
         <v>-99</v>
       </c>
       <c r="BT3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="BU3">
         <v>-99</v>
@@ -2979,7 +2356,7 @@
         <v>-99</v>
       </c>
       <c r="CB3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="CC3">
         <v>-99</v>
@@ -2994,7 +2371,7 @@
         <v>-99</v>
       </c>
       <c r="CG3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="CH3">
         <v>-99</v>
@@ -3111,7 +2488,7 @@
         <v>-99</v>
       </c>
       <c r="DT3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="DU3">
         <v>-99</v>
@@ -3141,7 +2518,7 @@
         <v>-99</v>
       </c>
       <c r="ED3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="EE3">
         <v>-99</v>
@@ -3150,26 +2527,26 @@
         <v>-99</v>
       </c>
       <c r="EG3" t="s">
+        <v>196</v>
+      </c>
+      <c r="EH3">
+        <v>-99</v>
+      </c>
+      <c r="EI3">
+        <v>-99</v>
+      </c>
+      <c r="EJ3" t="s">
+        <v>196</v>
+      </c>
+      <c r="EK3">
+        <v>-99</v>
+      </c>
+      <c r="EL3">
+        <v>-99</v>
+      </c>
+      <c r="EM3" t="s">
         <v>197</v>
       </c>
-      <c r="EH3">
-        <v>-99</v>
-      </c>
-      <c r="EI3">
-        <v>-99</v>
-      </c>
-      <c r="EJ3" t="s">
-        <v>197</v>
-      </c>
-      <c r="EK3">
-        <v>-99</v>
-      </c>
-      <c r="EL3">
-        <v>-99</v>
-      </c>
-      <c r="EM3" t="s">
-        <v>198</v>
-      </c>
       <c r="EN3">
         <v>-99</v>
       </c>
@@ -3177,7 +2554,7 @@
         <v>-99</v>
       </c>
       <c r="EP3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="EQ3">
         <v>-99</v>
@@ -3186,7 +2563,7 @@
         <v>-99</v>
       </c>
       <c r="ES3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="ET3">
         <v>-99</v>
@@ -3195,7 +2572,7 @@
         <v>-99</v>
       </c>
       <c r="EV3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="EW3">
         <v>-99</v>
@@ -3213,7 +2590,7 @@
         <v>-99</v>
       </c>
       <c r="FB3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="FC3">
         <v>-99</v>
@@ -3222,7 +2599,7 @@
         <v>-99</v>
       </c>
       <c r="FE3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="FF3">
         <v>-99</v>
@@ -3236,14 +2613,14 @@
         <v>21742527</v>
       </c>
       <c r="B4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C4" t="s">
         <v>207</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>208</v>
       </c>
-      <c r="D4" t="s">
-        <v>209</v>
-      </c>
       <c r="E4">
         <v>-99</v>
       </c>
@@ -3257,13 +2634,13 @@
         <v>-99</v>
       </c>
       <c r="I4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J4">
         <v>19</v>
       </c>
       <c r="K4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L4">
         <v>-99</v>
@@ -3275,13 +2652,13 @@
         <v>-99</v>
       </c>
       <c r="O4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="P4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="Q4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="R4">
         <v>-99</v>
@@ -3305,7 +2682,7 @@
         <v>-99</v>
       </c>
       <c r="Y4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Z4">
         <v>-99</v>
@@ -3332,46 +2709,46 @@
         <v>19</v>
       </c>
       <c r="AH4" t="s">
+        <v>171</v>
+      </c>
+      <c r="AI4" t="s">
         <v>172</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="AJ4" t="s">
         <v>173</v>
       </c>
-      <c r="AJ4" t="s">
+      <c r="AK4" t="s">
         <v>174</v>
       </c>
-      <c r="AK4" t="s">
+      <c r="AL4" t="s">
         <v>175</v>
       </c>
-      <c r="AL4" t="s">
+      <c r="AM4" t="s">
         <v>176</v>
       </c>
-      <c r="AM4" t="s">
+      <c r="AN4" t="s">
         <v>177</v>
       </c>
-      <c r="AN4" t="s">
+      <c r="AO4" t="s">
         <v>178</v>
       </c>
-      <c r="AO4" t="s">
+      <c r="AP4" t="s">
         <v>179</v>
       </c>
-      <c r="AP4" t="s">
+      <c r="AQ4" t="s">
         <v>180</v>
       </c>
-      <c r="AQ4" t="s">
-        <v>181</v>
-      </c>
       <c r="AR4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AS4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AT4">
         <v>-99</v>
       </c>
       <c r="AU4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AV4">
         <v>-99</v>
@@ -3407,7 +2784,7 @@
         <v>-99</v>
       </c>
       <c r="BG4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="BH4">
         <v>-99</v>
@@ -3446,7 +2823,7 @@
         <v>-99</v>
       </c>
       <c r="BT4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="BU4">
         <v>-99</v>
@@ -3470,7 +2847,7 @@
         <v>-99</v>
       </c>
       <c r="CB4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="CC4">
         <v>-99</v>
@@ -3485,7 +2862,7 @@
         <v>-99</v>
       </c>
       <c r="CG4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="CH4">
         <v>-99</v>
@@ -3602,7 +2979,7 @@
         <v>-99</v>
       </c>
       <c r="DT4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="DU4">
         <v>-99</v>
@@ -3632,7 +3009,7 @@
         <v>-99</v>
       </c>
       <c r="ED4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="EE4">
         <v>-99</v>
@@ -3641,26 +3018,26 @@
         <v>-99</v>
       </c>
       <c r="EG4" t="s">
+        <v>196</v>
+      </c>
+      <c r="EH4">
+        <v>-99</v>
+      </c>
+      <c r="EI4">
+        <v>-99</v>
+      </c>
+      <c r="EJ4" t="s">
+        <v>196</v>
+      </c>
+      <c r="EK4">
+        <v>-99</v>
+      </c>
+      <c r="EL4">
+        <v>-99</v>
+      </c>
+      <c r="EM4" t="s">
         <v>197</v>
       </c>
-      <c r="EH4">
-        <v>-99</v>
-      </c>
-      <c r="EI4">
-        <v>-99</v>
-      </c>
-      <c r="EJ4" t="s">
-        <v>197</v>
-      </c>
-      <c r="EK4">
-        <v>-99</v>
-      </c>
-      <c r="EL4">
-        <v>-99</v>
-      </c>
-      <c r="EM4" t="s">
-        <v>198</v>
-      </c>
       <c r="EN4">
         <v>-99</v>
       </c>
@@ -3668,7 +3045,7 @@
         <v>-99</v>
       </c>
       <c r="EP4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="EQ4">
         <v>-99</v>
@@ -3677,7 +3054,7 @@
         <v>-99</v>
       </c>
       <c r="ES4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="ET4">
         <v>-99</v>
@@ -3686,7 +3063,7 @@
         <v>-99</v>
       </c>
       <c r="EV4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="EW4">
         <v>-99</v>
@@ -3704,7 +3081,7 @@
         <v>-99</v>
       </c>
       <c r="FB4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="FC4">
         <v>-99</v>
@@ -3713,7 +3090,7 @@
         <v>-99</v>
       </c>
       <c r="FE4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="FF4">
         <v>-99</v>
@@ -3727,34 +3104,34 @@
         <v>27123476</v>
       </c>
       <c r="B5" t="s">
+        <v>213</v>
+      </c>
+      <c r="C5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D5" t="s">
         <v>214</v>
       </c>
-      <c r="C5" t="s">
-        <v>164</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="E5">
+        <v>-99</v>
+      </c>
+      <c r="F5">
+        <v>-99</v>
+      </c>
+      <c r="G5">
+        <v>-99</v>
+      </c>
+      <c r="H5">
+        <v>-99</v>
+      </c>
+      <c r="I5" t="s">
         <v>215</v>
-      </c>
-      <c r="E5">
-        <v>-99</v>
-      </c>
-      <c r="F5">
-        <v>-99</v>
-      </c>
-      <c r="G5">
-        <v>-99</v>
-      </c>
-      <c r="H5">
-        <v>-99</v>
-      </c>
-      <c r="I5" t="s">
-        <v>216</v>
       </c>
       <c r="J5">
         <v>6</v>
       </c>
       <c r="K5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L5">
         <v>1</v>
@@ -3763,16 +3140,16 @@
         <v>-99</v>
       </c>
       <c r="N5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="O5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="P5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="Q5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="R5">
         <v>-99</v>
@@ -3796,7 +3173,7 @@
         <v>-99</v>
       </c>
       <c r="Y5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Z5">
         <v>-99</v>
@@ -3823,148 +3200,148 @@
         <v>19</v>
       </c>
       <c r="AH5" t="s">
+        <v>171</v>
+      </c>
+      <c r="AI5" t="s">
         <v>172</v>
       </c>
-      <c r="AI5" t="s">
+      <c r="AJ5" t="s">
         <v>173</v>
       </c>
-      <c r="AJ5" t="s">
+      <c r="AK5" t="s">
         <v>174</v>
       </c>
-      <c r="AK5" t="s">
+      <c r="AL5" t="s">
         <v>175</v>
       </c>
-      <c r="AL5" t="s">
+      <c r="AM5" t="s">
         <v>176</v>
       </c>
-      <c r="AM5" t="s">
+      <c r="AN5" t="s">
         <v>177</v>
       </c>
-      <c r="AN5" t="s">
+      <c r="AO5" t="s">
         <v>178</v>
       </c>
-      <c r="AO5" t="s">
+      <c r="AP5" t="s">
         <v>179</v>
       </c>
-      <c r="AP5" t="s">
+      <c r="AQ5" t="s">
         <v>180</v>
       </c>
-      <c r="AQ5" t="s">
+      <c r="AR5" t="s">
         <v>181</v>
       </c>
-      <c r="AR5" t="s">
+      <c r="AS5" t="s">
         <v>182</v>
       </c>
-      <c r="AS5" t="s">
+      <c r="AT5">
+        <v>-99</v>
+      </c>
+      <c r="AU5" t="s">
         <v>183</v>
       </c>
-      <c r="AT5">
-        <v>-99</v>
-      </c>
-      <c r="AU5" t="s">
-        <v>184</v>
-      </c>
       <c r="AV5" t="s">
+        <v>171</v>
+      </c>
+      <c r="AW5" t="s">
         <v>172</v>
       </c>
-      <c r="AW5" t="s">
+      <c r="AX5" t="s">
         <v>173</v>
       </c>
-      <c r="AX5" t="s">
-        <v>174</v>
-      </c>
       <c r="AY5" t="s">
+        <v>217</v>
+      </c>
+      <c r="AZ5" t="s">
+        <v>185</v>
+      </c>
+      <c r="BA5" t="s">
         <v>218</v>
       </c>
-      <c r="AZ5" t="s">
-        <v>186</v>
-      </c>
-      <c r="BA5" t="s">
+      <c r="BB5" t="s">
         <v>219</v>
       </c>
-      <c r="BB5" t="s">
+      <c r="BC5" t="s">
         <v>220</v>
       </c>
-      <c r="BC5" t="s">
+      <c r="BD5" t="s">
         <v>221</v>
       </c>
-      <c r="BD5" t="s">
+      <c r="BE5" t="s">
         <v>222</v>
       </c>
-      <c r="BE5" t="s">
+      <c r="BF5" t="s">
+        <v>181</v>
+      </c>
+      <c r="BG5" t="s">
         <v>223</v>
       </c>
-      <c r="BF5" t="s">
-        <v>182</v>
-      </c>
-      <c r="BG5" t="s">
+      <c r="BH5">
+        <v>-99</v>
+      </c>
+      <c r="BI5">
+        <v>-99</v>
+      </c>
+      <c r="BJ5">
+        <v>-99</v>
+      </c>
+      <c r="BK5">
+        <v>-99</v>
+      </c>
+      <c r="BL5">
+        <v>-99</v>
+      </c>
+      <c r="BM5">
+        <v>-99</v>
+      </c>
+      <c r="BN5">
+        <v>-99</v>
+      </c>
+      <c r="BO5">
+        <v>-99</v>
+      </c>
+      <c r="BP5">
+        <v>-99</v>
+      </c>
+      <c r="BQ5">
+        <v>-99</v>
+      </c>
+      <c r="BR5">
+        <v>-99</v>
+      </c>
+      <c r="BS5">
+        <v>-99</v>
+      </c>
+      <c r="BT5" t="s">
+        <v>190</v>
+      </c>
+      <c r="BU5">
+        <v>-99</v>
+      </c>
+      <c r="BV5">
+        <v>-99</v>
+      </c>
+      <c r="BW5">
+        <v>-99</v>
+      </c>
+      <c r="BX5">
+        <v>-99</v>
+      </c>
+      <c r="BY5">
+        <v>-99</v>
+      </c>
+      <c r="BZ5" t="s">
+        <v>169</v>
+      </c>
+      <c r="CA5">
+        <v>-99</v>
+      </c>
+      <c r="CB5" t="s">
+        <v>169</v>
+      </c>
+      <c r="CC5" t="s">
         <v>224</v>
-      </c>
-      <c r="BH5">
-        <v>-99</v>
-      </c>
-      <c r="BI5">
-        <v>-99</v>
-      </c>
-      <c r="BJ5">
-        <v>-99</v>
-      </c>
-      <c r="BK5">
-        <v>-99</v>
-      </c>
-      <c r="BL5">
-        <v>-99</v>
-      </c>
-      <c r="BM5">
-        <v>-99</v>
-      </c>
-      <c r="BN5">
-        <v>-99</v>
-      </c>
-      <c r="BO5">
-        <v>-99</v>
-      </c>
-      <c r="BP5">
-        <v>-99</v>
-      </c>
-      <c r="BQ5">
-        <v>-99</v>
-      </c>
-      <c r="BR5">
-        <v>-99</v>
-      </c>
-      <c r="BS5">
-        <v>-99</v>
-      </c>
-      <c r="BT5" t="s">
-        <v>191</v>
-      </c>
-      <c r="BU5">
-        <v>-99</v>
-      </c>
-      <c r="BV5">
-        <v>-99</v>
-      </c>
-      <c r="BW5">
-        <v>-99</v>
-      </c>
-      <c r="BX5">
-        <v>-99</v>
-      </c>
-      <c r="BY5">
-        <v>-99</v>
-      </c>
-      <c r="BZ5" t="s">
-        <v>170</v>
-      </c>
-      <c r="CA5">
-        <v>-99</v>
-      </c>
-      <c r="CB5" t="s">
-        <v>170</v>
-      </c>
-      <c r="CC5" t="s">
-        <v>225</v>
       </c>
       <c r="CD5">
         <v>36</v>
@@ -3976,19 +3353,19 @@
         <v>-99</v>
       </c>
       <c r="CG5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="CH5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="CI5">
         <v>-99</v>
       </c>
       <c r="CJ5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="CK5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="CL5">
         <v>-99</v>
@@ -3997,13 +3374,13 @@
         <v>-99</v>
       </c>
       <c r="CN5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="CO5">
         <v>-99</v>
       </c>
       <c r="CP5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="CQ5">
         <v>-99</v>
@@ -4018,10 +3395,10 @@
         <v>-99</v>
       </c>
       <c r="CU5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="CV5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="CW5">
         <v>-99</v>
@@ -4033,7 +3410,7 @@
         <v>-99</v>
       </c>
       <c r="CZ5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="DA5">
         <v>-99</v>
@@ -4072,7 +3449,7 @@
         <v>-99</v>
       </c>
       <c r="DM5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="DN5">
         <v>-99</v>
@@ -4081,19 +3458,19 @@
         <v>-99</v>
       </c>
       <c r="DP5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="DQ5">
         <v>-99</v>
       </c>
       <c r="DR5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="DS5">
         <v>-99</v>
       </c>
       <c r="DT5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="DU5">
         <v>-99</v>
@@ -4105,82 +3482,82 @@
         <v>-99</v>
       </c>
       <c r="DX5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="DY5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="DZ5" t="s">
         <v>85</v>
       </c>
       <c r="EA5" t="s">
+        <v>226</v>
+      </c>
+      <c r="EB5">
+        <v>-99</v>
+      </c>
+      <c r="EC5">
+        <v>-99</v>
+      </c>
+      <c r="ED5" t="s">
+        <v>194</v>
+      </c>
+      <c r="EE5" t="s">
+        <v>195</v>
+      </c>
+      <c r="EF5">
+        <v>-99</v>
+      </c>
+      <c r="EG5" t="s">
+        <v>196</v>
+      </c>
+      <c r="EH5" t="s">
+        <v>195</v>
+      </c>
+      <c r="EI5">
+        <v>-99</v>
+      </c>
+      <c r="EJ5" t="s">
+        <v>196</v>
+      </c>
+      <c r="EK5" t="s">
+        <v>195</v>
+      </c>
+      <c r="EL5">
+        <v>-99</v>
+      </c>
+      <c r="EM5" t="s">
+        <v>197</v>
+      </c>
+      <c r="EN5" t="s">
         <v>227</v>
       </c>
-      <c r="EB5">
-        <v>-99</v>
-      </c>
-      <c r="EC5">
-        <v>-99</v>
-      </c>
-      <c r="ED5" t="s">
+      <c r="EO5">
+        <v>-99</v>
+      </c>
+      <c r="EP5" t="s">
+        <v>196</v>
+      </c>
+      <c r="EQ5" t="s">
         <v>195</v>
       </c>
-      <c r="EE5" t="s">
-        <v>196</v>
-      </c>
-      <c r="EF5">
-        <v>-99</v>
-      </c>
-      <c r="EG5" t="s">
-        <v>197</v>
-      </c>
-      <c r="EH5" t="s">
-        <v>196</v>
-      </c>
-      <c r="EI5">
-        <v>-99</v>
-      </c>
-      <c r="EJ5" t="s">
-        <v>197</v>
-      </c>
-      <c r="EK5" t="s">
-        <v>196</v>
-      </c>
-      <c r="EL5">
-        <v>-99</v>
-      </c>
-      <c r="EM5" t="s">
-        <v>198</v>
-      </c>
-      <c r="EN5" t="s">
+      <c r="ER5">
+        <v>-99</v>
+      </c>
+      <c r="ES5" t="s">
+        <v>199</v>
+      </c>
+      <c r="ET5" t="s">
         <v>228</v>
       </c>
-      <c r="EO5">
-        <v>-99</v>
-      </c>
-      <c r="EP5" t="s">
-        <v>197</v>
-      </c>
-      <c r="EQ5" t="s">
-        <v>196</v>
-      </c>
-      <c r="ER5">
-        <v>-99</v>
-      </c>
-      <c r="ES5" t="s">
-        <v>200</v>
-      </c>
-      <c r="ET5" t="s">
+      <c r="EU5">
+        <v>-99</v>
+      </c>
+      <c r="EV5" t="s">
+        <v>201</v>
+      </c>
+      <c r="EW5" t="s">
         <v>229</v>
-      </c>
-      <c r="EU5">
-        <v>-99</v>
-      </c>
-      <c r="EV5" t="s">
-        <v>202</v>
-      </c>
-      <c r="EW5" t="s">
-        <v>230</v>
       </c>
       <c r="EX5">
         <v>-99</v>
@@ -4195,7 +3572,7 @@
         <v>-99</v>
       </c>
       <c r="FB5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="FC5">
         <v>-99</v>
@@ -4204,7 +3581,7 @@
         <v>-99</v>
       </c>
       <c r="FE5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="FF5">
         <v>-99</v>
@@ -4218,14 +3595,14 @@
         <v>27123476</v>
       </c>
       <c r="B6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C6" t="s">
+        <v>163</v>
+      </c>
+      <c r="D6" t="s">
         <v>214</v>
       </c>
-      <c r="C6" t="s">
-        <v>164</v>
-      </c>
-      <c r="D6" t="s">
-        <v>215</v>
-      </c>
       <c r="E6">
         <v>-99</v>
       </c>
@@ -4239,13 +3616,13 @@
         <v>-99</v>
       </c>
       <c r="I6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J6">
         <v>9</v>
       </c>
       <c r="K6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L6">
         <v>1</v>
@@ -4254,16 +3631,16 @@
         <v>-99</v>
       </c>
       <c r="N6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="O6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="P6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="Q6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="R6">
         <v>-99</v>
@@ -4287,7 +3664,7 @@
         <v>-99</v>
       </c>
       <c r="Y6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Z6">
         <v>-99</v>
@@ -4314,46 +3691,46 @@
         <v>19</v>
       </c>
       <c r="AH6" t="s">
+        <v>171</v>
+      </c>
+      <c r="AI6" t="s">
         <v>172</v>
       </c>
-      <c r="AI6" t="s">
+      <c r="AJ6" t="s">
         <v>173</v>
       </c>
-      <c r="AJ6" t="s">
+      <c r="AK6" t="s">
         <v>174</v>
       </c>
-      <c r="AK6" t="s">
+      <c r="AL6" t="s">
         <v>175</v>
       </c>
-      <c r="AL6" t="s">
+      <c r="AM6" t="s">
         <v>176</v>
       </c>
-      <c r="AM6" t="s">
+      <c r="AN6" t="s">
         <v>177</v>
       </c>
-      <c r="AN6" t="s">
+      <c r="AO6" t="s">
         <v>178</v>
       </c>
-      <c r="AO6" t="s">
+      <c r="AP6" t="s">
         <v>179</v>
       </c>
-      <c r="AP6" t="s">
+      <c r="AQ6" t="s">
         <v>180</v>
       </c>
-      <c r="AQ6" t="s">
-        <v>181</v>
-      </c>
       <c r="AR6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AS6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AT6">
         <v>-99</v>
       </c>
       <c r="AU6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AV6">
         <v>-99</v>
@@ -4389,7 +3766,7 @@
         <v>-99</v>
       </c>
       <c r="BG6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="BH6">
         <v>-99</v>
@@ -4428,7 +3805,7 @@
         <v>-99</v>
       </c>
       <c r="BT6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="BU6">
         <v>-99</v>
@@ -4440,46 +3817,46 @@
         <v>-99</v>
       </c>
       <c r="BX6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="BY6">
         <v>-99</v>
       </c>
       <c r="BZ6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="CA6">
         <v>-99</v>
       </c>
       <c r="CB6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="CC6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="CD6">
         <v>36</v>
       </c>
       <c r="CE6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="CF6">
         <v>36</v>
       </c>
       <c r="CG6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="CH6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="CI6">
         <v>-99</v>
       </c>
       <c r="CJ6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="CK6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="CL6">
         <v>-99</v>
@@ -4488,7 +3865,7 @@
         <v>-99</v>
       </c>
       <c r="CN6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="CO6">
         <v>-99</v>
@@ -4509,13 +3886,13 @@
         <v>-99</v>
       </c>
       <c r="CU6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="CV6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="CW6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="CX6">
         <v>-99</v>
@@ -4524,7 +3901,7 @@
         <v>-99</v>
       </c>
       <c r="CZ6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="DA6">
         <v>-99</v>
@@ -4551,7 +3928,7 @@
         <v>-99</v>
       </c>
       <c r="DI6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="DJ6">
         <v>-99</v>
@@ -4560,19 +3937,19 @@
         <v>-99</v>
       </c>
       <c r="DL6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="DM6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="DN6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="DO6">
         <v>-99</v>
       </c>
       <c r="DP6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="DQ6">
         <v>-99</v>
@@ -4584,7 +3961,7 @@
         <v>-99</v>
       </c>
       <c r="DT6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="DU6">
         <v>-99</v>
@@ -4596,7 +3973,7 @@
         <v>-99</v>
       </c>
       <c r="DX6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="DY6">
         <v>-99</v>
@@ -4614,7 +3991,7 @@
         <v>-99</v>
       </c>
       <c r="ED6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="EE6">
         <v>-99</v>
@@ -4623,26 +4000,26 @@
         <v>-99</v>
       </c>
       <c r="EG6" t="s">
+        <v>196</v>
+      </c>
+      <c r="EH6">
+        <v>-99</v>
+      </c>
+      <c r="EI6">
+        <v>-99</v>
+      </c>
+      <c r="EJ6" t="s">
+        <v>196</v>
+      </c>
+      <c r="EK6">
+        <v>-99</v>
+      </c>
+      <c r="EL6">
+        <v>-99</v>
+      </c>
+      <c r="EM6" t="s">
         <v>197</v>
       </c>
-      <c r="EH6">
-        <v>-99</v>
-      </c>
-      <c r="EI6">
-        <v>-99</v>
-      </c>
-      <c r="EJ6" t="s">
-        <v>197</v>
-      </c>
-      <c r="EK6">
-        <v>-99</v>
-      </c>
-      <c r="EL6">
-        <v>-99</v>
-      </c>
-      <c r="EM6" t="s">
-        <v>198</v>
-      </c>
       <c r="EN6">
         <v>-99</v>
       </c>
@@ -4650,7 +4027,7 @@
         <v>-99</v>
       </c>
       <c r="EP6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="EQ6">
         <v>-99</v>
@@ -4659,7 +4036,7 @@
         <v>-99</v>
       </c>
       <c r="ES6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="ET6">
         <v>-99</v>
@@ -4668,7 +4045,7 @@
         <v>-99</v>
       </c>
       <c r="EV6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="EW6">
         <v>-99</v>
@@ -4686,7 +4063,7 @@
         <v>-99</v>
       </c>
       <c r="FB6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="FC6">
         <v>-99</v>
@@ -4695,7 +4072,7 @@
         <v>-99</v>
       </c>
       <c r="FE6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="FF6">
         <v>-99</v>
@@ -4709,14 +4086,14 @@
         <v>27123476</v>
       </c>
       <c r="B7" t="s">
+        <v>213</v>
+      </c>
+      <c r="C7" t="s">
+        <v>163</v>
+      </c>
+      <c r="D7" t="s">
         <v>214</v>
       </c>
-      <c r="C7" t="s">
-        <v>164</v>
-      </c>
-      <c r="D7" t="s">
-        <v>215</v>
-      </c>
       <c r="E7">
         <v>-99</v>
       </c>
@@ -4730,13 +4107,13 @@
         <v>-99</v>
       </c>
       <c r="I7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J7">
         <v>17</v>
       </c>
       <c r="K7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L7">
         <v>1</v>
@@ -4745,16 +4122,16 @@
         <v>-99</v>
       </c>
       <c r="N7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="O7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="P7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="R7">
         <v>-99</v>
@@ -4778,7 +4155,7 @@
         <v>-99</v>
       </c>
       <c r="Y7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Z7">
         <v>-99</v>
@@ -4805,83 +4182,83 @@
         <v>19</v>
       </c>
       <c r="AH7" t="s">
+        <v>171</v>
+      </c>
+      <c r="AI7" t="s">
         <v>172</v>
       </c>
-      <c r="AI7" t="s">
+      <c r="AJ7" t="s">
         <v>173</v>
       </c>
-      <c r="AJ7" t="s">
+      <c r="AK7" t="s">
         <v>174</v>
       </c>
-      <c r="AK7" t="s">
+      <c r="AL7" t="s">
         <v>175</v>
       </c>
-      <c r="AL7" t="s">
+      <c r="AM7" t="s">
         <v>176</v>
       </c>
-      <c r="AM7" t="s">
+      <c r="AN7" t="s">
         <v>177</v>
       </c>
-      <c r="AN7" t="s">
+      <c r="AO7" t="s">
         <v>178</v>
       </c>
-      <c r="AO7" t="s">
+      <c r="AP7" t="s">
         <v>179</v>
       </c>
-      <c r="AP7" t="s">
+      <c r="AQ7" t="s">
         <v>180</v>
       </c>
-      <c r="AQ7" t="s">
+      <c r="AR7" t="s">
         <v>181</v>
       </c>
-      <c r="AR7" t="s">
+      <c r="AS7" t="s">
         <v>182</v>
       </c>
-      <c r="AS7" t="s">
+      <c r="AT7">
+        <v>-99</v>
+      </c>
+      <c r="AU7" t="s">
         <v>183</v>
       </c>
-      <c r="AT7">
-        <v>-99</v>
-      </c>
-      <c r="AU7" t="s">
-        <v>184</v>
-      </c>
       <c r="AV7" t="s">
+        <v>171</v>
+      </c>
+      <c r="AW7" t="s">
         <v>172</v>
       </c>
-      <c r="AW7" t="s">
+      <c r="AX7" t="s">
         <v>173</v>
       </c>
-      <c r="AX7" t="s">
-        <v>174</v>
-      </c>
       <c r="AY7" t="s">
+        <v>217</v>
+      </c>
+      <c r="AZ7" t="s">
+        <v>185</v>
+      </c>
+      <c r="BA7" t="s">
         <v>218</v>
       </c>
-      <c r="AZ7" t="s">
-        <v>186</v>
-      </c>
-      <c r="BA7" t="s">
+      <c r="BB7" t="s">
         <v>219</v>
       </c>
-      <c r="BB7" t="s">
+      <c r="BC7" t="s">
         <v>220</v>
       </c>
-      <c r="BC7" t="s">
+      <c r="BD7" t="s">
         <v>221</v>
       </c>
-      <c r="BD7" t="s">
+      <c r="BE7" t="s">
         <v>222</v>
       </c>
-      <c r="BE7" t="s">
+      <c r="BF7" t="s">
+        <v>181</v>
+      </c>
+      <c r="BG7" t="s">
         <v>223</v>
       </c>
-      <c r="BF7" t="s">
-        <v>182</v>
-      </c>
-      <c r="BG7" t="s">
-        <v>224</v>
-      </c>
       <c r="BH7">
         <v>-99</v>
       </c>
@@ -4919,106 +4296,106 @@
         <v>-99</v>
       </c>
       <c r="BT7" t="s">
+        <v>190</v>
+      </c>
+      <c r="BU7">
+        <v>-99</v>
+      </c>
+      <c r="BV7">
+        <v>-99</v>
+      </c>
+      <c r="BW7">
+        <v>-99</v>
+      </c>
+      <c r="BX7" t="s">
+        <v>169</v>
+      </c>
+      <c r="BY7">
+        <v>-99</v>
+      </c>
+      <c r="BZ7" t="s">
+        <v>169</v>
+      </c>
+      <c r="CA7">
+        <v>-99</v>
+      </c>
+      <c r="CB7" t="s">
+        <v>169</v>
+      </c>
+      <c r="CC7">
+        <v>-99</v>
+      </c>
+      <c r="CD7">
+        <v>-99</v>
+      </c>
+      <c r="CE7">
+        <v>-99</v>
+      </c>
+      <c r="CF7">
+        <v>-99</v>
+      </c>
+      <c r="CG7" t="s">
+        <v>169</v>
+      </c>
+      <c r="CH7">
+        <v>-99</v>
+      </c>
+      <c r="CI7">
+        <v>-99</v>
+      </c>
+      <c r="CJ7" t="s">
+        <v>169</v>
+      </c>
+      <c r="CK7" t="s">
+        <v>169</v>
+      </c>
+      <c r="CL7">
+        <v>-99</v>
+      </c>
+      <c r="CM7">
+        <v>-99</v>
+      </c>
+      <c r="CN7">
+        <v>-99</v>
+      </c>
+      <c r="CO7">
+        <v>-99</v>
+      </c>
+      <c r="CP7">
+        <v>-99</v>
+      </c>
+      <c r="CQ7">
+        <v>-99</v>
+      </c>
+      <c r="CR7">
+        <v>-99</v>
+      </c>
+      <c r="CS7">
+        <v>-99</v>
+      </c>
+      <c r="CT7">
+        <v>-99</v>
+      </c>
+      <c r="CU7" t="s">
+        <v>169</v>
+      </c>
+      <c r="CV7" t="s">
+        <v>169</v>
+      </c>
+      <c r="CW7">
+        <v>-99</v>
+      </c>
+      <c r="CX7">
+        <v>-99</v>
+      </c>
+      <c r="CY7">
+        <v>-99</v>
+      </c>
+      <c r="CZ7" t="s">
         <v>191</v>
       </c>
-      <c r="BU7">
-        <v>-99</v>
-      </c>
-      <c r="BV7">
-        <v>-99</v>
-      </c>
-      <c r="BW7">
-        <v>-99</v>
-      </c>
-      <c r="BX7" t="s">
-        <v>170</v>
-      </c>
-      <c r="BY7">
-        <v>-99</v>
-      </c>
-      <c r="BZ7" t="s">
-        <v>170</v>
-      </c>
-      <c r="CA7">
-        <v>-99</v>
-      </c>
-      <c r="CB7" t="s">
-        <v>170</v>
-      </c>
-      <c r="CC7">
-        <v>-99</v>
-      </c>
-      <c r="CD7">
-        <v>-99</v>
-      </c>
-      <c r="CE7">
-        <v>-99</v>
-      </c>
-      <c r="CF7">
-        <v>-99</v>
-      </c>
-      <c r="CG7" t="s">
-        <v>170</v>
-      </c>
-      <c r="CH7">
-        <v>-99</v>
-      </c>
-      <c r="CI7">
-        <v>-99</v>
-      </c>
-      <c r="CJ7" t="s">
-        <v>170</v>
-      </c>
-      <c r="CK7" t="s">
-        <v>170</v>
-      </c>
-      <c r="CL7">
-        <v>-99</v>
-      </c>
-      <c r="CM7">
-        <v>-99</v>
-      </c>
-      <c r="CN7">
-        <v>-99</v>
-      </c>
-      <c r="CO7">
-        <v>-99</v>
-      </c>
-      <c r="CP7">
-        <v>-99</v>
-      </c>
-      <c r="CQ7">
-        <v>-99</v>
-      </c>
-      <c r="CR7">
-        <v>-99</v>
-      </c>
-      <c r="CS7">
-        <v>-99</v>
-      </c>
-      <c r="CT7">
-        <v>-99</v>
-      </c>
-      <c r="CU7" t="s">
-        <v>170</v>
-      </c>
-      <c r="CV7" t="s">
-        <v>170</v>
-      </c>
-      <c r="CW7">
-        <v>-99</v>
-      </c>
-      <c r="CX7">
-        <v>-99</v>
-      </c>
-      <c r="CY7">
-        <v>-99</v>
-      </c>
-      <c r="CZ7" t="s">
-        <v>192</v>
-      </c>
       <c r="DA7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="DB7">
         <v>-99</v>
@@ -5051,10 +4428,10 @@
         <v>-99</v>
       </c>
       <c r="DL7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="DM7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="DN7">
         <v>-99</v>
@@ -5075,7 +4452,7 @@
         <v>-99</v>
       </c>
       <c r="DT7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="DU7">
         <v>-99</v>
@@ -5087,7 +4464,7 @@
         <v>-99</v>
       </c>
       <c r="DX7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="DY7">
         <v>-99</v>
@@ -5105,64 +4482,64 @@
         <v>-99</v>
       </c>
       <c r="ED7" t="s">
+        <v>194</v>
+      </c>
+      <c r="EE7" t="s">
         <v>195</v>
       </c>
-      <c r="EE7" t="s">
+      <c r="EF7">
+        <v>-99</v>
+      </c>
+      <c r="EG7" t="s">
         <v>196</v>
       </c>
-      <c r="EF7">
-        <v>-99</v>
-      </c>
-      <c r="EG7" t="s">
+      <c r="EH7" t="s">
+        <v>195</v>
+      </c>
+      <c r="EI7">
+        <v>-99</v>
+      </c>
+      <c r="EJ7" t="s">
+        <v>196</v>
+      </c>
+      <c r="EK7" t="s">
+        <v>195</v>
+      </c>
+      <c r="EL7">
+        <v>-99</v>
+      </c>
+      <c r="EM7" t="s">
         <v>197</v>
       </c>
-      <c r="EH7" t="s">
+      <c r="EN7" t="s">
+        <v>227</v>
+      </c>
+      <c r="EO7">
+        <v>-99</v>
+      </c>
+      <c r="EP7" t="s">
         <v>196</v>
       </c>
-      <c r="EI7">
-        <v>-99</v>
-      </c>
-      <c r="EJ7" t="s">
-        <v>197</v>
-      </c>
-      <c r="EK7" t="s">
-        <v>196</v>
-      </c>
-      <c r="EL7">
-        <v>-99</v>
-      </c>
-      <c r="EM7" t="s">
-        <v>198</v>
-      </c>
-      <c r="EN7" t="s">
+      <c r="EQ7" t="s">
+        <v>195</v>
+      </c>
+      <c r="ER7">
+        <v>-99</v>
+      </c>
+      <c r="ES7" t="s">
+        <v>199</v>
+      </c>
+      <c r="ET7" t="s">
         <v>228</v>
       </c>
-      <c r="EO7">
-        <v>-99</v>
-      </c>
-      <c r="EP7" t="s">
-        <v>197</v>
-      </c>
-      <c r="EQ7" t="s">
-        <v>196</v>
-      </c>
-      <c r="ER7">
-        <v>-99</v>
-      </c>
-      <c r="ES7" t="s">
-        <v>200</v>
-      </c>
-      <c r="ET7" t="s">
+      <c r="EU7">
+        <v>-99</v>
+      </c>
+      <c r="EV7" t="s">
+        <v>201</v>
+      </c>
+      <c r="EW7" t="s">
         <v>229</v>
-      </c>
-      <c r="EU7">
-        <v>-99</v>
-      </c>
-      <c r="EV7" t="s">
-        <v>202</v>
-      </c>
-      <c r="EW7" t="s">
-        <v>230</v>
       </c>
       <c r="EX7">
         <v>-99</v>
@@ -5177,7 +4554,7 @@
         <v>-99</v>
       </c>
       <c r="FB7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="FC7">
         <v>-99</v>
@@ -5186,7 +4563,7 @@
         <v>-99</v>
       </c>
       <c r="FE7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="FF7">
         <v>-99</v>
@@ -5200,14 +4577,14 @@
         <v>27123476</v>
       </c>
       <c r="B8" t="s">
+        <v>213</v>
+      </c>
+      <c r="C8" t="s">
+        <v>163</v>
+      </c>
+      <c r="D8" t="s">
         <v>214</v>
       </c>
-      <c r="C8" t="s">
-        <v>164</v>
-      </c>
-      <c r="D8" t="s">
-        <v>215</v>
-      </c>
       <c r="E8">
         <v>-99</v>
       </c>
@@ -5221,13 +4598,13 @@
         <v>-99</v>
       </c>
       <c r="I8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J8">
         <v>19</v>
       </c>
       <c r="K8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L8">
         <v>1</v>
@@ -5236,16 +4613,16 @@
         <v>-99</v>
       </c>
       <c r="N8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="O8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="P8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="R8">
         <v>-99</v>
@@ -5269,7 +4646,7 @@
         <v>-99</v>
       </c>
       <c r="Y8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Z8">
         <v>-99</v>
@@ -5296,46 +4673,46 @@
         <v>19</v>
       </c>
       <c r="AH8" t="s">
+        <v>171</v>
+      </c>
+      <c r="AI8" t="s">
         <v>172</v>
       </c>
-      <c r="AI8" t="s">
+      <c r="AJ8" t="s">
         <v>173</v>
       </c>
-      <c r="AJ8" t="s">
+      <c r="AK8" t="s">
         <v>174</v>
       </c>
-      <c r="AK8" t="s">
+      <c r="AL8" t="s">
         <v>175</v>
       </c>
-      <c r="AL8" t="s">
+      <c r="AM8" t="s">
         <v>176</v>
       </c>
-      <c r="AM8" t="s">
+      <c r="AN8" t="s">
         <v>177</v>
       </c>
-      <c r="AN8" t="s">
+      <c r="AO8" t="s">
         <v>178</v>
       </c>
-      <c r="AO8" t="s">
+      <c r="AP8" t="s">
         <v>179</v>
       </c>
-      <c r="AP8" t="s">
+      <c r="AQ8" t="s">
         <v>180</v>
       </c>
-      <c r="AQ8" t="s">
-        <v>181</v>
-      </c>
       <c r="AR8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AS8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AT8">
         <v>-99</v>
       </c>
       <c r="AU8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AV8">
         <v>-99</v>
@@ -5371,214 +4748,214 @@
         <v>-99</v>
       </c>
       <c r="BG8" t="s">
+        <v>190</v>
+      </c>
+      <c r="BH8">
+        <v>-99</v>
+      </c>
+      <c r="BI8">
+        <v>-99</v>
+      </c>
+      <c r="BJ8">
+        <v>-99</v>
+      </c>
+      <c r="BK8">
+        <v>-99</v>
+      </c>
+      <c r="BL8">
+        <v>-99</v>
+      </c>
+      <c r="BM8">
+        <v>-99</v>
+      </c>
+      <c r="BN8">
+        <v>-99</v>
+      </c>
+      <c r="BO8">
+        <v>-99</v>
+      </c>
+      <c r="BP8">
+        <v>-99</v>
+      </c>
+      <c r="BQ8">
+        <v>-99</v>
+      </c>
+      <c r="BR8">
+        <v>-99</v>
+      </c>
+      <c r="BS8">
+        <v>-99</v>
+      </c>
+      <c r="BT8" t="s">
+        <v>190</v>
+      </c>
+      <c r="BU8">
+        <v>-99</v>
+      </c>
+      <c r="BV8">
+        <v>-99</v>
+      </c>
+      <c r="BW8">
+        <v>-99</v>
+      </c>
+      <c r="BX8" t="s">
+        <v>169</v>
+      </c>
+      <c r="BY8" t="s">
+        <v>169</v>
+      </c>
+      <c r="BZ8" t="s">
+        <v>169</v>
+      </c>
+      <c r="CA8">
+        <v>-99</v>
+      </c>
+      <c r="CB8" t="s">
+        <v>169</v>
+      </c>
+      <c r="CC8">
+        <v>-99</v>
+      </c>
+      <c r="CD8">
+        <v>-99</v>
+      </c>
+      <c r="CE8">
+        <v>-99</v>
+      </c>
+      <c r="CF8">
+        <v>-99</v>
+      </c>
+      <c r="CG8" t="s">
+        <v>169</v>
+      </c>
+      <c r="CH8">
+        <v>-99</v>
+      </c>
+      <c r="CI8">
+        <v>-99</v>
+      </c>
+      <c r="CJ8">
+        <v>-99</v>
+      </c>
+      <c r="CK8">
+        <v>-99</v>
+      </c>
+      <c r="CL8">
+        <v>-99</v>
+      </c>
+      <c r="CM8">
+        <v>-99</v>
+      </c>
+      <c r="CN8" t="s">
+        <v>169</v>
+      </c>
+      <c r="CO8">
+        <v>-99</v>
+      </c>
+      <c r="CP8">
+        <v>-99</v>
+      </c>
+      <c r="CQ8">
+        <v>-99</v>
+      </c>
+      <c r="CR8">
+        <v>-99</v>
+      </c>
+      <c r="CS8">
+        <v>-99</v>
+      </c>
+      <c r="CT8">
+        <v>-99</v>
+      </c>
+      <c r="CU8" t="s">
+        <v>169</v>
+      </c>
+      <c r="CV8" t="s">
+        <v>169</v>
+      </c>
+      <c r="CW8" t="s">
+        <v>169</v>
+      </c>
+      <c r="CX8">
+        <v>-99</v>
+      </c>
+      <c r="CY8">
+        <v>-99</v>
+      </c>
+      <c r="CZ8" t="s">
+        <v>169</v>
+      </c>
+      <c r="DA8">
+        <v>-99</v>
+      </c>
+      <c r="DB8">
+        <v>-99</v>
+      </c>
+      <c r="DC8">
+        <v>-99</v>
+      </c>
+      <c r="DD8">
+        <v>-99</v>
+      </c>
+      <c r="DE8">
+        <v>-99</v>
+      </c>
+      <c r="DF8">
+        <v>-99</v>
+      </c>
+      <c r="DG8">
+        <v>-99</v>
+      </c>
+      <c r="DH8">
+        <v>-99</v>
+      </c>
+      <c r="DI8">
+        <v>-99</v>
+      </c>
+      <c r="DJ8">
+        <v>-99</v>
+      </c>
+      <c r="DK8">
+        <v>-99</v>
+      </c>
+      <c r="DL8">
+        <v>-99</v>
+      </c>
+      <c r="DM8">
+        <v>-99</v>
+      </c>
+      <c r="DN8">
+        <v>-99</v>
+      </c>
+      <c r="DO8">
+        <v>-99</v>
+      </c>
+      <c r="DP8">
+        <v>-99</v>
+      </c>
+      <c r="DQ8">
+        <v>-99</v>
+      </c>
+      <c r="DR8" t="s">
+        <v>169</v>
+      </c>
+      <c r="DS8">
+        <v>-99</v>
+      </c>
+      <c r="DT8" t="s">
+        <v>169</v>
+      </c>
+      <c r="DU8">
+        <v>-99</v>
+      </c>
+      <c r="DV8">
+        <v>-99</v>
+      </c>
+      <c r="DW8">
+        <v>-99</v>
+      </c>
+      <c r="DX8" t="s">
         <v>191</v>
-      </c>
-      <c r="BH8">
-        <v>-99</v>
-      </c>
-      <c r="BI8">
-        <v>-99</v>
-      </c>
-      <c r="BJ8">
-        <v>-99</v>
-      </c>
-      <c r="BK8">
-        <v>-99</v>
-      </c>
-      <c r="BL8">
-        <v>-99</v>
-      </c>
-      <c r="BM8">
-        <v>-99</v>
-      </c>
-      <c r="BN8">
-        <v>-99</v>
-      </c>
-      <c r="BO8">
-        <v>-99</v>
-      </c>
-      <c r="BP8">
-        <v>-99</v>
-      </c>
-      <c r="BQ8">
-        <v>-99</v>
-      </c>
-      <c r="BR8">
-        <v>-99</v>
-      </c>
-      <c r="BS8">
-        <v>-99</v>
-      </c>
-      <c r="BT8" t="s">
-        <v>191</v>
-      </c>
-      <c r="BU8">
-        <v>-99</v>
-      </c>
-      <c r="BV8">
-        <v>-99</v>
-      </c>
-      <c r="BW8">
-        <v>-99</v>
-      </c>
-      <c r="BX8" t="s">
-        <v>170</v>
-      </c>
-      <c r="BY8" t="s">
-        <v>170</v>
-      </c>
-      <c r="BZ8" t="s">
-        <v>170</v>
-      </c>
-      <c r="CA8">
-        <v>-99</v>
-      </c>
-      <c r="CB8" t="s">
-        <v>170</v>
-      </c>
-      <c r="CC8">
-        <v>-99</v>
-      </c>
-      <c r="CD8">
-        <v>-99</v>
-      </c>
-      <c r="CE8">
-        <v>-99</v>
-      </c>
-      <c r="CF8">
-        <v>-99</v>
-      </c>
-      <c r="CG8" t="s">
-        <v>170</v>
-      </c>
-      <c r="CH8">
-        <v>-99</v>
-      </c>
-      <c r="CI8">
-        <v>-99</v>
-      </c>
-      <c r="CJ8">
-        <v>-99</v>
-      </c>
-      <c r="CK8">
-        <v>-99</v>
-      </c>
-      <c r="CL8">
-        <v>-99</v>
-      </c>
-      <c r="CM8">
-        <v>-99</v>
-      </c>
-      <c r="CN8" t="s">
-        <v>170</v>
-      </c>
-      <c r="CO8">
-        <v>-99</v>
-      </c>
-      <c r="CP8">
-        <v>-99</v>
-      </c>
-      <c r="CQ8">
-        <v>-99</v>
-      </c>
-      <c r="CR8">
-        <v>-99</v>
-      </c>
-      <c r="CS8">
-        <v>-99</v>
-      </c>
-      <c r="CT8">
-        <v>-99</v>
-      </c>
-      <c r="CU8" t="s">
-        <v>170</v>
-      </c>
-      <c r="CV8" t="s">
-        <v>170</v>
-      </c>
-      <c r="CW8" t="s">
-        <v>170</v>
-      </c>
-      <c r="CX8">
-        <v>-99</v>
-      </c>
-      <c r="CY8">
-        <v>-99</v>
-      </c>
-      <c r="CZ8" t="s">
-        <v>170</v>
-      </c>
-      <c r="DA8">
-        <v>-99</v>
-      </c>
-      <c r="DB8">
-        <v>-99</v>
-      </c>
-      <c r="DC8">
-        <v>-99</v>
-      </c>
-      <c r="DD8">
-        <v>-99</v>
-      </c>
-      <c r="DE8">
-        <v>-99</v>
-      </c>
-      <c r="DF8">
-        <v>-99</v>
-      </c>
-      <c r="DG8">
-        <v>-99</v>
-      </c>
-      <c r="DH8">
-        <v>-99</v>
-      </c>
-      <c r="DI8">
-        <v>-99</v>
-      </c>
-      <c r="DJ8">
-        <v>-99</v>
-      </c>
-      <c r="DK8">
-        <v>-99</v>
-      </c>
-      <c r="DL8">
-        <v>-99</v>
-      </c>
-      <c r="DM8">
-        <v>-99</v>
-      </c>
-      <c r="DN8">
-        <v>-99</v>
-      </c>
-      <c r="DO8">
-        <v>-99</v>
-      </c>
-      <c r="DP8">
-        <v>-99</v>
-      </c>
-      <c r="DQ8">
-        <v>-99</v>
-      </c>
-      <c r="DR8" t="s">
-        <v>170</v>
-      </c>
-      <c r="DS8">
-        <v>-99</v>
-      </c>
-      <c r="DT8" t="s">
-        <v>170</v>
-      </c>
-      <c r="DU8">
-        <v>-99</v>
-      </c>
-      <c r="DV8">
-        <v>-99</v>
-      </c>
-      <c r="DW8">
-        <v>-99</v>
-      </c>
-      <c r="DX8" t="s">
-        <v>192</v>
       </c>
       <c r="DY8">
         <v>-99</v>
@@ -5596,7 +4973,7 @@
         <v>-99</v>
       </c>
       <c r="ED8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="EE8">
         <v>-99</v>
@@ -5605,26 +4982,26 @@
         <v>-99</v>
       </c>
       <c r="EG8" t="s">
+        <v>196</v>
+      </c>
+      <c r="EH8">
+        <v>-99</v>
+      </c>
+      <c r="EI8">
+        <v>-99</v>
+      </c>
+      <c r="EJ8" t="s">
+        <v>196</v>
+      </c>
+      <c r="EK8">
+        <v>-99</v>
+      </c>
+      <c r="EL8">
+        <v>-99</v>
+      </c>
+      <c r="EM8" t="s">
         <v>197</v>
       </c>
-      <c r="EH8">
-        <v>-99</v>
-      </c>
-      <c r="EI8">
-        <v>-99</v>
-      </c>
-      <c r="EJ8" t="s">
-        <v>197</v>
-      </c>
-      <c r="EK8">
-        <v>-99</v>
-      </c>
-      <c r="EL8">
-        <v>-99</v>
-      </c>
-      <c r="EM8" t="s">
-        <v>198</v>
-      </c>
       <c r="EN8">
         <v>-99</v>
       </c>
@@ -5632,7 +5009,7 @@
         <v>-99</v>
       </c>
       <c r="EP8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="EQ8">
         <v>-99</v>
@@ -5641,7 +5018,7 @@
         <v>-99</v>
       </c>
       <c r="ES8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="ET8">
         <v>-99</v>
@@ -5650,7 +5027,7 @@
         <v>-99</v>
       </c>
       <c r="EV8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="EW8">
         <v>-99</v>
@@ -5668,7 +5045,7 @@
         <v>-99</v>
       </c>
       <c r="FB8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="FC8">
         <v>-99</v>
@@ -5677,7 +5054,7 @@
         <v>-99</v>
       </c>
       <c r="FE8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="FF8">
         <v>-99</v>
@@ -5691,34 +5068,34 @@
         <v>31785030</v>
       </c>
       <c r="B9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C9" t="s">
+        <v>163</v>
+      </c>
+      <c r="D9" t="s">
         <v>235</v>
       </c>
-      <c r="C9" t="s">
-        <v>164</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E9">
+        <v>-99</v>
+      </c>
+      <c r="F9">
+        <v>-99</v>
+      </c>
+      <c r="G9">
+        <v>-99</v>
+      </c>
+      <c r="H9">
+        <v>-99</v>
+      </c>
+      <c r="I9" t="s">
+        <v>230</v>
+      </c>
+      <c r="J9" t="s">
         <v>236</v>
       </c>
-      <c r="E9">
-        <v>-99</v>
-      </c>
-      <c r="F9">
-        <v>-99</v>
-      </c>
-      <c r="G9">
-        <v>-99</v>
-      </c>
-      <c r="H9">
-        <v>-99</v>
-      </c>
-      <c r="I9" t="s">
-        <v>231</v>
-      </c>
-      <c r="J9" t="s">
-        <v>237</v>
-      </c>
       <c r="K9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L9">
         <v>-99</v>
@@ -5727,19 +5104,19 @@
         <v>-99</v>
       </c>
       <c r="N9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="O9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="P9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="Q9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="R9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="S9">
         <v>-99</v>
@@ -5760,7 +5137,7 @@
         <v>-99</v>
       </c>
       <c r="Y9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Z9">
         <v>59</v>
@@ -5787,83 +5164,83 @@
         <v>19</v>
       </c>
       <c r="AH9" t="s">
+        <v>171</v>
+      </c>
+      <c r="AI9" t="s">
         <v>172</v>
       </c>
-      <c r="AI9" t="s">
+      <c r="AJ9" t="s">
         <v>173</v>
       </c>
-      <c r="AJ9" t="s">
+      <c r="AK9" t="s">
         <v>174</v>
       </c>
-      <c r="AK9" t="s">
+      <c r="AL9" t="s">
         <v>175</v>
       </c>
-      <c r="AL9" t="s">
+      <c r="AM9" t="s">
         <v>176</v>
       </c>
-      <c r="AM9" t="s">
+      <c r="AN9" t="s">
         <v>177</v>
       </c>
-      <c r="AN9" t="s">
+      <c r="AO9" t="s">
         <v>178</v>
       </c>
-      <c r="AO9" t="s">
+      <c r="AP9" t="s">
         <v>179</v>
       </c>
-      <c r="AP9" t="s">
+      <c r="AQ9" t="s">
         <v>180</v>
       </c>
-      <c r="AQ9" t="s">
+      <c r="AR9" t="s">
         <v>181</v>
       </c>
-      <c r="AR9" t="s">
+      <c r="AS9" t="s">
         <v>182</v>
       </c>
-      <c r="AS9" t="s">
+      <c r="AT9">
+        <v>-99</v>
+      </c>
+      <c r="AU9" t="s">
         <v>183</v>
       </c>
-      <c r="AT9">
-        <v>-99</v>
-      </c>
-      <c r="AU9" t="s">
-        <v>184</v>
-      </c>
       <c r="AV9" t="s">
+        <v>171</v>
+      </c>
+      <c r="AW9" t="s">
         <v>172</v>
       </c>
-      <c r="AW9" t="s">
+      <c r="AX9" t="s">
         <v>173</v>
       </c>
-      <c r="AX9" t="s">
-        <v>174</v>
-      </c>
       <c r="AY9" t="s">
+        <v>217</v>
+      </c>
+      <c r="AZ9" t="s">
+        <v>185</v>
+      </c>
+      <c r="BA9" t="s">
         <v>218</v>
       </c>
-      <c r="AZ9" t="s">
-        <v>186</v>
-      </c>
-      <c r="BA9" t="s">
+      <c r="BB9" t="s">
         <v>219</v>
       </c>
-      <c r="BB9" t="s">
+      <c r="BC9" t="s">
         <v>220</v>
       </c>
-      <c r="BC9" t="s">
+      <c r="BD9" t="s">
         <v>221</v>
       </c>
-      <c r="BD9" t="s">
+      <c r="BE9" t="s">
         <v>222</v>
       </c>
-      <c r="BE9" t="s">
+      <c r="BF9" t="s">
+        <v>181</v>
+      </c>
+      <c r="BG9" t="s">
         <v>223</v>
       </c>
-      <c r="BF9" t="s">
-        <v>182</v>
-      </c>
-      <c r="BG9" t="s">
-        <v>224</v>
-      </c>
       <c r="BH9">
         <v>-99</v>
       </c>
@@ -5901,7 +5278,7 @@
         <v>-99</v>
       </c>
       <c r="BT9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="BU9">
         <v>-99</v>
@@ -5919,13 +5296,13 @@
         <v>-99</v>
       </c>
       <c r="BZ9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="CA9">
         <v>-99</v>
       </c>
       <c r="CB9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="CC9">
         <v>-99</v>
@@ -5940,19 +5317,19 @@
         <v>-99</v>
       </c>
       <c r="CG9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="CH9">
         <v>-99</v>
       </c>
       <c r="CI9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="CJ9">
         <v>-99</v>
       </c>
       <c r="CK9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="CL9">
         <v>-99</v>
@@ -5961,7 +5338,7 @@
         <v>-99</v>
       </c>
       <c r="CN9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="CO9">
         <v>-99</v>
@@ -6045,19 +5422,19 @@
         <v>-99</v>
       </c>
       <c r="DP9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="DQ9">
         <v>-99</v>
       </c>
       <c r="DR9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="DS9">
         <v>-99</v>
       </c>
       <c r="DT9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="DU9">
         <v>-99</v>
@@ -6087,64 +5464,64 @@
         <v>-99</v>
       </c>
       <c r="ED9" t="s">
+        <v>194</v>
+      </c>
+      <c r="EE9" t="s">
         <v>195</v>
       </c>
-      <c r="EE9" t="s">
+      <c r="EF9">
+        <v>-99</v>
+      </c>
+      <c r="EG9" t="s">
         <v>196</v>
       </c>
-      <c r="EF9">
-        <v>-99</v>
-      </c>
-      <c r="EG9" t="s">
+      <c r="EH9" t="s">
+        <v>195</v>
+      </c>
+      <c r="EI9">
+        <v>-99</v>
+      </c>
+      <c r="EJ9" t="s">
+        <v>196</v>
+      </c>
+      <c r="EK9" t="s">
+        <v>195</v>
+      </c>
+      <c r="EL9">
+        <v>-99</v>
+      </c>
+      <c r="EM9" t="s">
         <v>197</v>
       </c>
-      <c r="EH9" t="s">
+      <c r="EN9" t="s">
+        <v>227</v>
+      </c>
+      <c r="EO9">
+        <v>-99</v>
+      </c>
+      <c r="EP9" t="s">
         <v>196</v>
       </c>
-      <c r="EI9">
-        <v>-99</v>
-      </c>
-      <c r="EJ9" t="s">
-        <v>197</v>
-      </c>
-      <c r="EK9" t="s">
-        <v>196</v>
-      </c>
-      <c r="EL9">
-        <v>-99</v>
-      </c>
-      <c r="EM9" t="s">
-        <v>198</v>
-      </c>
-      <c r="EN9" t="s">
+      <c r="EQ9" t="s">
+        <v>195</v>
+      </c>
+      <c r="ER9">
+        <v>-99</v>
+      </c>
+      <c r="ES9" t="s">
+        <v>199</v>
+      </c>
+      <c r="ET9" t="s">
         <v>228</v>
       </c>
-      <c r="EO9">
-        <v>-99</v>
-      </c>
-      <c r="EP9" t="s">
-        <v>197</v>
-      </c>
-      <c r="EQ9" t="s">
-        <v>196</v>
-      </c>
-      <c r="ER9">
-        <v>-99</v>
-      </c>
-      <c r="ES9" t="s">
-        <v>200</v>
-      </c>
-      <c r="ET9" t="s">
+      <c r="EU9">
+        <v>-99</v>
+      </c>
+      <c r="EV9" t="s">
+        <v>201</v>
+      </c>
+      <c r="EW9" t="s">
         <v>229</v>
-      </c>
-      <c r="EU9">
-        <v>-99</v>
-      </c>
-      <c r="EV9" t="s">
-        <v>202</v>
-      </c>
-      <c r="EW9" t="s">
-        <v>230</v>
       </c>
       <c r="EX9">
         <v>-99</v>
@@ -6159,7 +5536,7 @@
         <v>-99</v>
       </c>
       <c r="FB9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="FC9">
         <v>-99</v>
@@ -6168,7 +5545,7 @@
         <v>-99</v>
       </c>
       <c r="FE9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="FF9">
         <v>-99</v>
@@ -6182,34 +5559,34 @@
         <v>36087397</v>
       </c>
       <c r="B10" t="s">
+        <v>237</v>
+      </c>
+      <c r="C10" t="s">
         <v>238</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10">
+        <v>-99</v>
+      </c>
+      <c r="E10">
+        <v>-99</v>
+      </c>
+      <c r="F10">
+        <v>-99</v>
+      </c>
+      <c r="G10">
+        <v>-99</v>
+      </c>
+      <c r="H10">
+        <v>-99</v>
+      </c>
+      <c r="I10" t="s">
         <v>239</v>
-      </c>
-      <c r="D10">
-        <v>-99</v>
-      </c>
-      <c r="E10">
-        <v>-99</v>
-      </c>
-      <c r="F10">
-        <v>-99</v>
-      </c>
-      <c r="G10">
-        <v>-99</v>
-      </c>
-      <c r="H10">
-        <v>-99</v>
-      </c>
-      <c r="I10" t="s">
-        <v>240</v>
       </c>
       <c r="J10">
         <v>8</v>
       </c>
       <c r="K10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L10">
         <v>-99</v>
@@ -6218,16 +5595,16 @@
         <v>-99</v>
       </c>
       <c r="N10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="O10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="P10">
         <v>-99</v>
       </c>
       <c r="Q10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="R10">
         <v>-99</v>
@@ -6251,7 +5628,7 @@
         <v>-99</v>
       </c>
       <c r="Y10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Z10">
         <v>-99</v>
@@ -6278,46 +5655,46 @@
         <v>19</v>
       </c>
       <c r="AH10" t="s">
+        <v>171</v>
+      </c>
+      <c r="AI10" t="s">
         <v>172</v>
       </c>
-      <c r="AI10" t="s">
+      <c r="AJ10" t="s">
         <v>173</v>
       </c>
-      <c r="AJ10" t="s">
+      <c r="AK10" t="s">
         <v>174</v>
       </c>
-      <c r="AK10" t="s">
+      <c r="AL10" t="s">
         <v>175</v>
       </c>
-      <c r="AL10" t="s">
+      <c r="AM10" t="s">
         <v>176</v>
       </c>
-      <c r="AM10" t="s">
+      <c r="AN10" t="s">
         <v>177</v>
       </c>
-      <c r="AN10" t="s">
+      <c r="AO10" t="s">
         <v>178</v>
       </c>
-      <c r="AO10" t="s">
+      <c r="AP10" t="s">
         <v>179</v>
       </c>
-      <c r="AP10" t="s">
+      <c r="AQ10" t="s">
         <v>180</v>
       </c>
-      <c r="AQ10" t="s">
-        <v>181</v>
-      </c>
       <c r="AR10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AS10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AT10">
         <v>-99</v>
       </c>
       <c r="AU10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AV10">
         <v>-99</v>
@@ -6353,7 +5730,7 @@
         <v>-99</v>
       </c>
       <c r="BG10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="BH10">
         <v>-99</v>
@@ -6392,7 +5769,7 @@
         <v>-99</v>
       </c>
       <c r="BT10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="BU10">
         <v>-99</v>
@@ -6416,7 +5793,7 @@
         <v>-99</v>
       </c>
       <c r="CB10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="CC10">
         <v>-99</v>
@@ -6431,7 +5808,7 @@
         <v>-99</v>
       </c>
       <c r="CG10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="CH10">
         <v>-99</v>
@@ -6548,7 +5925,7 @@
         <v>-99</v>
       </c>
       <c r="DT10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="DU10">
         <v>-99</v>
@@ -6578,7 +5955,7 @@
         <v>-99</v>
       </c>
       <c r="ED10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="EE10">
         <v>-99</v>
@@ -6587,26 +5964,26 @@
         <v>-99</v>
       </c>
       <c r="EG10" t="s">
+        <v>196</v>
+      </c>
+      <c r="EH10">
+        <v>-99</v>
+      </c>
+      <c r="EI10">
+        <v>-99</v>
+      </c>
+      <c r="EJ10" t="s">
+        <v>196</v>
+      </c>
+      <c r="EK10">
+        <v>-99</v>
+      </c>
+      <c r="EL10">
+        <v>-99</v>
+      </c>
+      <c r="EM10" t="s">
         <v>197</v>
       </c>
-      <c r="EH10">
-        <v>-99</v>
-      </c>
-      <c r="EI10">
-        <v>-99</v>
-      </c>
-      <c r="EJ10" t="s">
-        <v>197</v>
-      </c>
-      <c r="EK10">
-        <v>-99</v>
-      </c>
-      <c r="EL10">
-        <v>-99</v>
-      </c>
-      <c r="EM10" t="s">
-        <v>198</v>
-      </c>
       <c r="EN10">
         <v>-99</v>
       </c>
@@ -6614,7 +5991,7 @@
         <v>-99</v>
       </c>
       <c r="EP10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="EQ10">
         <v>-99</v>
@@ -6623,7 +6000,7 @@
         <v>-99</v>
       </c>
       <c r="ES10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="ET10">
         <v>-99</v>
@@ -6632,7 +6009,7 @@
         <v>-99</v>
       </c>
       <c r="EV10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="EW10">
         <v>-99</v>
@@ -6650,7 +6027,7 @@
         <v>-99</v>
       </c>
       <c r="FB10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="FC10">
         <v>-99</v>
@@ -6659,7 +6036,7 @@
         <v>-99</v>
       </c>
       <c r="FE10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="FF10">
         <v>-99</v>
@@ -6670,6 +6047,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>